<commit_message>
Adding SpreadSheets under Sprint1 folder
</commit_message>
<xml_diff>
--- a/sprint 1/Meeting Minutes.xlsx
+++ b/sprint 1/Meeting Minutes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveconcordia-my.sharepoint.com/personal/h_aitidi_live_concordia_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A4EC3AC-74BD-4217-B80F-8D9F04BF9BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4C679DB-320B-4860-8FA1-B2865CB99CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F085AB1-CC62-4F65-BB42-6A16AAA4B60C}"/>
   </bookViews>
@@ -71,7 +71,13 @@
     <t>Houssam Ait Idir 40155665</t>
   </si>
   <si>
-    <t>Houssam had work all day he couldn't attend</t>
+    <t>we need to edit the Readme and include everyone Background
+-we need to divide the teams
+-we need to come up with the User Stories
+-we need to derive tasks from those User Stories
+-we created the Meeting Minutes Spread Sheet
+-we will creat the Member Contribution for each memeber
+-we need to plan for next sprint</t>
   </si>
   <si>
     <t>7/2/2024 From 6:00PM to 7:00PM (1 hours)</t>
@@ -510,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB572D5-F24F-4266-AB53-31A69FCFFF61}">
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -520,7 +526,7 @@
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
     <col min="7" max="7" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
   </cols>
@@ -578,7 +584,7 @@
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -601,20 +607,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b9246430-805d-4990-8c6c-7658ea52df43" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b9246430-805d-4990-8c6c-7658ea52df43" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -774,11 +780,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C682CB3-B94B-4D95-8521-F96752B03DE9}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96F69750-3FC9-4C88-898D-08E08111D695}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C682CB3-B94B-4D95-8521-F96752B03DE9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>